<commit_message>
241021, oxford modified sunday 22:00
</commit_message>
<xml_diff>
--- a/R/data/quiz241021.xlsx
+++ b/R/data/quiz241021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kwlee/Dropbox/내 Mac (Kee-Won의 MacBook Air)/Documents/class202402/R/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5C26BEF-9A36-C840-BCF7-0974DD8D92EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A6E5F81-980A-3B47-967E-BE7C19CA0E2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="35520" yWindow="1380" windowWidth="44180" windowHeight="23100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6655" uniqueCount="1457">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7415" uniqueCount="1607">
   <si>
     <t>타임스탬프</t>
   </si>
@@ -4392,6 +4392,456 @@
   </si>
   <si>
     <t>정연주</t>
+  </si>
+  <si>
+    <t>haeun_ob@naver.com</t>
+  </si>
+  <si>
+    <t>박하은</t>
+  </si>
+  <si>
+    <t>skaskgus@gmail.com</t>
+  </si>
+  <si>
+    <t>남나현</t>
+  </si>
+  <si>
+    <t>jongjongsook@naver.com</t>
+  </si>
+  <si>
+    <t>김종숙</t>
+  </si>
+  <si>
+    <t>coreykang3@naver.com</t>
+  </si>
+  <si>
+    <t>반도체공학</t>
+  </si>
+  <si>
+    <t>강동훈</t>
+  </si>
+  <si>
+    <t>mkjk1227@naver.com</t>
+  </si>
+  <si>
+    <t>정민기</t>
+  </si>
+  <si>
+    <t>mire030503@gmail.com</t>
+  </si>
+  <si>
+    <t>디지털미디어콘텐츠 학과</t>
+  </si>
+  <si>
+    <t>김원형</t>
+  </si>
+  <si>
+    <t>dngud4@naver.com</t>
+  </si>
+  <si>
+    <t>이우형</t>
+  </si>
+  <si>
+    <t>lsd5741@naver.com</t>
+  </si>
+  <si>
+    <t>이소담</t>
+  </si>
+  <si>
+    <t>wpghks1145@gmail.com</t>
+  </si>
+  <si>
+    <t>박제환</t>
+  </si>
+  <si>
+    <t>wendy040507@naver.com</t>
+  </si>
+  <si>
+    <t>tmddl3538@naver.com</t>
+  </si>
+  <si>
+    <t>kte1785@naver.com</t>
+  </si>
+  <si>
+    <t>chltjdnjs2421@naver.com</t>
+  </si>
+  <si>
+    <t>최서원</t>
+  </si>
+  <si>
+    <t>sonsumin0304@naver.com</t>
+  </si>
+  <si>
+    <t>손수민</t>
+  </si>
+  <si>
+    <t>dream03064@gmail.com</t>
+  </si>
+  <si>
+    <t>오채연</t>
+  </si>
+  <si>
+    <t>ueusudjsjsksksk@gmail.com</t>
+  </si>
+  <si>
+    <t>강동현</t>
+  </si>
+  <si>
+    <t>hjjj051014@naver.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">안효정 </t>
+  </si>
+  <si>
+    <t>jisung050407@naver.com</t>
+  </si>
+  <si>
+    <t>김지성</t>
+  </si>
+  <si>
+    <t>ysuyes@gmail.com</t>
+  </si>
+  <si>
+    <t>윤승욱</t>
+  </si>
+  <si>
+    <t>oh4559@gmail.com</t>
+  </si>
+  <si>
+    <t>권오현</t>
+  </si>
+  <si>
+    <t>xx0911ram1@gmail.com</t>
+  </si>
+  <si>
+    <t>글로벌비즈니스</t>
+  </si>
+  <si>
+    <t>정하람</t>
+  </si>
+  <si>
+    <t>min010417@gmail.com</t>
+  </si>
+  <si>
+    <t>강채민</t>
+  </si>
+  <si>
+    <t>tlsh1282@naver.com</t>
+  </si>
+  <si>
+    <t>융합관광경영</t>
+  </si>
+  <si>
+    <t>원세한</t>
+  </si>
+  <si>
+    <t>chlwnstn777@naver.com</t>
+  </si>
+  <si>
+    <t>최준수</t>
+  </si>
+  <si>
+    <t>khj000818@naver.com</t>
+  </si>
+  <si>
+    <t>강현준</t>
+  </si>
+  <si>
+    <t>jjhjo2070@gmail.com</t>
+  </si>
+  <si>
+    <t>조정훈</t>
+  </si>
+  <si>
+    <t>yoosun91124@gmail.com</t>
+  </si>
+  <si>
+    <t>박윤선</t>
+  </si>
+  <si>
+    <t>skyhaneul0910@naver.com</t>
+  </si>
+  <si>
+    <t>권하늘</t>
+  </si>
+  <si>
+    <t>hiday_516@naver.com</t>
+  </si>
+  <si>
+    <t>양희지</t>
+  </si>
+  <si>
+    <t>tkddnt0608@gmail.com</t>
+  </si>
+  <si>
+    <t>유상욱</t>
+  </si>
+  <si>
+    <t>hanca0607@naver.com</t>
+  </si>
+  <si>
+    <t>한채아</t>
+  </si>
+  <si>
+    <t>nurasun02@gmail.com</t>
+  </si>
+  <si>
+    <t>이주연</t>
+  </si>
+  <si>
+    <t>seokwony123@gmail.com</t>
+  </si>
+  <si>
+    <t>양석원</t>
+  </si>
+  <si>
+    <t>jaekyung001203@gmail.com</t>
+  </si>
+  <si>
+    <t>안재경</t>
+  </si>
+  <si>
+    <t>uek2002@naver.com</t>
+  </si>
+  <si>
+    <t>김기조</t>
+  </si>
+  <si>
+    <t>xluwq264@gmail.com</t>
+  </si>
+  <si>
+    <t>주시은</t>
+  </si>
+  <si>
+    <t>opix97@naver.com</t>
+  </si>
+  <si>
+    <t>조성훈</t>
+  </si>
+  <si>
+    <t>yerimyerim11@naver.com</t>
+  </si>
+  <si>
+    <t>syuniw26@gmail.com</t>
+  </si>
+  <si>
+    <t>이서윤</t>
+  </si>
+  <si>
+    <t>20222849@hallym.ac.kr</t>
+  </si>
+  <si>
+    <t>한애진</t>
+  </si>
+  <si>
+    <t>seoeun2003@naver.com</t>
+  </si>
+  <si>
+    <t>최서은</t>
+  </si>
+  <si>
+    <t>yule240110@gmail.com</t>
+  </si>
+  <si>
+    <t>조율</t>
+  </si>
+  <si>
+    <t>u2fjfjrjdjjr2@naver.com</t>
+  </si>
+  <si>
+    <t>기소연</t>
+  </si>
+  <si>
+    <t>xhddlfqnxkr@naver.com</t>
+  </si>
+  <si>
+    <t>김보경</t>
+  </si>
+  <si>
+    <t>hcheon27@gmail.com</t>
+  </si>
+  <si>
+    <t>천하윤</t>
+  </si>
+  <si>
+    <t>mnnnmm22@naver.com</t>
+  </si>
+  <si>
+    <t>고현아</t>
+  </si>
+  <si>
+    <t>tlqpfldkghfk@gmail.com</t>
+  </si>
+  <si>
+    <t>jinsol.oh84@gmail.com</t>
+  </si>
+  <si>
+    <t>오진솔</t>
+  </si>
+  <si>
+    <t>hsbg1118@gmail.com</t>
+  </si>
+  <si>
+    <t>전희성</t>
+  </si>
+  <si>
+    <t>tommy580134@naver.com</t>
+  </si>
+  <si>
+    <t>예준원</t>
+  </si>
+  <si>
+    <t>5tmddk@naver.com</t>
+  </si>
+  <si>
+    <t>최승아</t>
+  </si>
+  <si>
+    <t>jiurim0316@naver.com</t>
+  </si>
+  <si>
+    <t>지우림</t>
+  </si>
+  <si>
+    <t>ndd1016@gmail.com</t>
+  </si>
+  <si>
+    <t>최형렬</t>
+  </si>
+  <si>
+    <t>h20216510@glab.hallym.ac.kr</t>
+  </si>
+  <si>
+    <t>AI기술경영융합전공</t>
+  </si>
+  <si>
+    <t>김지인</t>
+  </si>
+  <si>
+    <t>sua@hallym.ac.kr</t>
+  </si>
+  <si>
+    <t>김수아</t>
+  </si>
+  <si>
+    <t>dw060419@naver.com</t>
+  </si>
+  <si>
+    <t>김도원</t>
+  </si>
+  <si>
+    <t>p060627@naver.com</t>
+  </si>
+  <si>
+    <t>박찬혁</t>
+  </si>
+  <si>
+    <t>soomin0282@gmail.com</t>
+  </si>
+  <si>
+    <t>lsarang1311@gmail.com</t>
+  </si>
+  <si>
+    <t>이사랑</t>
+  </si>
+  <si>
+    <t>gordon0625@naver.com</t>
+  </si>
+  <si>
+    <t>김승재</t>
+  </si>
+  <si>
+    <t>ghkdxo2003@gmail.com</t>
+  </si>
+  <si>
+    <t>황이준</t>
+  </si>
+  <si>
+    <t>kentoku0901@naver.com</t>
+  </si>
+  <si>
+    <t>사회복지</t>
+  </si>
+  <si>
+    <t>김헌덕</t>
+  </si>
+  <si>
+    <t>sasa8294@naver.com</t>
+  </si>
+  <si>
+    <t>신승환</t>
+  </si>
+  <si>
+    <t>dkdud4750@naver.com</t>
+  </si>
+  <si>
+    <t>양아영</t>
+  </si>
+  <si>
+    <t>dbsduwls691@naver.com</t>
+  </si>
+  <si>
+    <t>윤여진</t>
+  </si>
+  <si>
+    <t>nye3796@gmail.com</t>
+  </si>
+  <si>
+    <t>노예은</t>
+  </si>
+  <si>
+    <t>featherkim@naver.com</t>
+  </si>
+  <si>
+    <t>김향수</t>
+  </si>
+  <si>
+    <t>dahyeony410@gmail.com</t>
+  </si>
+  <si>
+    <t>윤다현</t>
+  </si>
+  <si>
+    <t>wjdtn2445@naver.com</t>
+  </si>
+  <si>
+    <t>이정수</t>
+  </si>
+  <si>
+    <t>bigeyejimmy1@naver.com</t>
+  </si>
+  <si>
+    <t>wkdgotqlc@gmail.com</t>
+  </si>
+  <si>
+    <t>장햇빛</t>
+  </si>
+  <si>
+    <t>cardinal0507@gmail.com</t>
+  </si>
+  <si>
+    <t>김수환</t>
+  </si>
+  <si>
+    <t>dojunc1@gmail.com</t>
+  </si>
+  <si>
+    <t>차도준</t>
+  </si>
+  <si>
+    <t>ism050204@naver.com</t>
+  </si>
+  <si>
+    <t>sky0219msh@naver.com</t>
+  </si>
+  <si>
+    <t>최하늘</t>
+  </si>
+  <si>
+    <t>shimyuna14@gmail.com</t>
+  </si>
+  <si>
+    <t>심유나</t>
   </si>
 </sst>
 </file>
@@ -4817,7 +5267,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Form_Responses1" displayName="Form_Responses1" ref="A1:O665" headerRowCount="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Form_Responses1" displayName="Form_Responses1" ref="A1:O741" headerRowCount="0">
   <tableColumns count="15">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Column1"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Column2"/>
@@ -5045,11 +5495,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:O665"/>
+  <dimension ref="A1:O741"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A623" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D670" sqref="D670"/>
+      <pane ySplit="1" topLeftCell="A700" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B747" sqref="B747"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -30334,9 +30784,6 @@
       <c r="I665" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="J665" s="20"/>
-      <c r="K665" s="20"/>
-      <c r="L665" s="20"/>
       <c r="M665" s="14" t="s">
         <v>27</v>
       </c>
@@ -30346,6 +30793,2900 @@
       <c r="O665" s="15" t="s">
         <v>57</v>
       </c>
+    </row>
+    <row r="666" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A666" s="4">
+        <v>45599.814243298606</v>
+      </c>
+      <c r="B666" s="5" t="s">
+        <v>1457</v>
+      </c>
+      <c r="C666" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D666" s="5">
+        <v>20222327</v>
+      </c>
+      <c r="E666" s="5" t="s">
+        <v>1458</v>
+      </c>
+      <c r="F666" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G666" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="H666" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I666" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="M666" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="N666" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="O666" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="667" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A667" s="7">
+        <v>45599.814933506947</v>
+      </c>
+      <c r="B667" s="8" t="s">
+        <v>1459</v>
+      </c>
+      <c r="C667" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="D667" s="8">
+        <v>20202324</v>
+      </c>
+      <c r="E667" s="8" t="s">
+        <v>1460</v>
+      </c>
+      <c r="F667" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G667" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H667" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="I667" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="J667" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="K667" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="L667" s="8" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="668" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A668" s="4">
+        <v>45599.814991539351</v>
+      </c>
+      <c r="B668" s="5" t="s">
+        <v>1461</v>
+      </c>
+      <c r="C668" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D668" s="5">
+        <v>20243613</v>
+      </c>
+      <c r="E668" s="5" t="s">
+        <v>1462</v>
+      </c>
+      <c r="F668" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G668" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H668" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I668" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="M668" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="N668" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="O668" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="669" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A669" s="7">
+        <v>45599.815416898149</v>
+      </c>
+      <c r="B669" s="8" t="s">
+        <v>1463</v>
+      </c>
+      <c r="C669" s="8" t="s">
+        <v>1464</v>
+      </c>
+      <c r="D669" s="8">
+        <v>20233301</v>
+      </c>
+      <c r="E669" s="8" t="s">
+        <v>1465</v>
+      </c>
+      <c r="F669" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="G669" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="H669" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="I669" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="M669" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="N669" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="O669" s="9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="670" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A670" s="4">
+        <v>45599.815790231485</v>
+      </c>
+      <c r="B670" s="5" t="s">
+        <v>1466</v>
+      </c>
+      <c r="C670" s="5" t="s">
+        <v>1466</v>
+      </c>
+      <c r="D670" s="5">
+        <v>20212840</v>
+      </c>
+      <c r="E670" s="5" t="s">
+        <v>1467</v>
+      </c>
+      <c r="F670" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G670" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H670" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I670" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="J670" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="K670" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="L670" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="671" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A671" s="7">
+        <v>45599.819280601849</v>
+      </c>
+      <c r="B671" s="8" t="s">
+        <v>1468</v>
+      </c>
+      <c r="C671" s="8" t="s">
+        <v>1469</v>
+      </c>
+      <c r="D671" s="8">
+        <v>20222514</v>
+      </c>
+      <c r="E671" s="8" t="s">
+        <v>1470</v>
+      </c>
+      <c r="F671" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G671" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H671" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="I671" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="J671" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="K671" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="L671" s="8" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="672" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A672" s="4">
+        <v>45599.819711168981</v>
+      </c>
+      <c r="B672" s="5" t="s">
+        <v>1471</v>
+      </c>
+      <c r="C672" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D672" s="5">
+        <v>20222424</v>
+      </c>
+      <c r="E672" s="5" t="s">
+        <v>1472</v>
+      </c>
+      <c r="F672" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G672" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="H672" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I672" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="J672" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K672" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L672" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="673" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A673" s="7">
+        <v>45599.823633090273</v>
+      </c>
+      <c r="B673" s="8" t="s">
+        <v>1473</v>
+      </c>
+      <c r="C673" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="D673" s="8">
+        <v>20242225</v>
+      </c>
+      <c r="E673" s="8" t="s">
+        <v>1474</v>
+      </c>
+      <c r="F673" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G673" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H673" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I673" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="M673" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="N673" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="O673" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="674" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A674" s="4">
+        <v>45599.826860173613</v>
+      </c>
+      <c r="B674" s="5" t="s">
+        <v>1475</v>
+      </c>
+      <c r="C674" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="D674" s="5">
+        <v>20201046</v>
+      </c>
+      <c r="E674" s="5" t="s">
+        <v>1476</v>
+      </c>
+      <c r="F674" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G674" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H674" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I674" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="J674" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K674" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L674" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="675" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A675" s="7">
+        <v>45599.832906967597</v>
+      </c>
+      <c r="B675" s="8" t="s">
+        <v>1477</v>
+      </c>
+      <c r="C675" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="D675" s="8">
+        <v>20243002</v>
+      </c>
+      <c r="E675" s="8" t="s">
+        <v>878</v>
+      </c>
+      <c r="F675" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="G675" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H675" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="I675" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="J675" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="K675" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="L675" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="676" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A676" s="4">
+        <v>45599.837630567126</v>
+      </c>
+      <c r="B676" s="5" t="s">
+        <v>1478</v>
+      </c>
+      <c r="C676" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="D676" s="5">
+        <v>20227037</v>
+      </c>
+      <c r="E676" s="5" t="s">
+        <v>1306</v>
+      </c>
+      <c r="F676" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G676" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H676" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I676" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="J676" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K676" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L676" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="677" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A677" s="7">
+        <v>45599.838494502314</v>
+      </c>
+      <c r="B677" s="8" t="s">
+        <v>1479</v>
+      </c>
+      <c r="C677" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="D677" s="8">
+        <v>20243913</v>
+      </c>
+      <c r="E677" s="8" t="s">
+        <v>786</v>
+      </c>
+      <c r="F677" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G677" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="H677" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="I677" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="M677" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="N677" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="O677" s="9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="678" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A678" s="4">
+        <v>45599.840309780091</v>
+      </c>
+      <c r="B678" s="5" t="s">
+        <v>1480</v>
+      </c>
+      <c r="C678" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="D678" s="5">
+        <v>20242848</v>
+      </c>
+      <c r="E678" s="5" t="s">
+        <v>1481</v>
+      </c>
+      <c r="F678" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G678" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H678" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="I678" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="M678" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="N678" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="O678" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="679" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A679" s="7">
+        <v>45599.844793344906</v>
+      </c>
+      <c r="B679" s="8" t="s">
+        <v>1482</v>
+      </c>
+      <c r="C679" s="8" t="s">
+        <v>264</v>
+      </c>
+      <c r="D679" s="8">
+        <v>20226748</v>
+      </c>
+      <c r="E679" s="8" t="s">
+        <v>1483</v>
+      </c>
+      <c r="F679" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G679" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="H679" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I679" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="J679" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="K679" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="L679" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="680" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A680" s="4">
+        <v>45599.847778923606</v>
+      </c>
+      <c r="B680" s="5" t="s">
+        <v>1484</v>
+      </c>
+      <c r="C680" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="D680" s="5">
+        <v>20243927</v>
+      </c>
+      <c r="E680" s="5" t="s">
+        <v>1485</v>
+      </c>
+      <c r="F680" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G680" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H680" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I680" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="J680" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="K680" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="L680" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="681" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A681" s="7">
+        <v>45599.848217164355</v>
+      </c>
+      <c r="B681" s="8" t="s">
+        <v>1486</v>
+      </c>
+      <c r="C681" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="D681" s="8">
+        <v>20245102</v>
+      </c>
+      <c r="E681" s="8" t="s">
+        <v>1487</v>
+      </c>
+      <c r="F681" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G681" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H681" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I681" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="M681" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="N681" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="O681" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="682" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A682" s="4">
+        <v>45599.848885069441</v>
+      </c>
+      <c r="B682" s="5" t="s">
+        <v>1488</v>
+      </c>
+      <c r="C682" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="D682" s="5">
+        <v>20243628</v>
+      </c>
+      <c r="E682" s="5" t="s">
+        <v>1489</v>
+      </c>
+      <c r="F682" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="G682" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H682" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="I682" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="M682" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="N682" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="O682" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="683" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A683" s="7">
+        <v>45599.849018831017</v>
+      </c>
+      <c r="B683" s="8" t="s">
+        <v>1490</v>
+      </c>
+      <c r="C683" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="D683" s="8">
+        <v>20242212</v>
+      </c>
+      <c r="E683" s="8" t="s">
+        <v>1491</v>
+      </c>
+      <c r="F683" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G683" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H683" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="I683" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="J683" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="K683" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="L683" s="8" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="684" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A684" s="4">
+        <v>45599.849033958337</v>
+      </c>
+      <c r="B684" s="5" t="s">
+        <v>1492</v>
+      </c>
+      <c r="C684" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D684" s="5">
+        <v>20242992</v>
+      </c>
+      <c r="E684" s="5" t="s">
+        <v>1493</v>
+      </c>
+      <c r="F684" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G684" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H684" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I684" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="J684" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K684" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L684" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="685" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A685" s="7">
+        <v>45599.850783541668</v>
+      </c>
+      <c r="B685" s="8" t="s">
+        <v>1494</v>
+      </c>
+      <c r="C685" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="D685" s="8">
+        <v>20215108</v>
+      </c>
+      <c r="E685" s="8" t="s">
+        <v>1495</v>
+      </c>
+      <c r="F685" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G685" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H685" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="I685" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="J685" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="K685" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="L685" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="686" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A686" s="4">
+        <v>45599.852150983796</v>
+      </c>
+      <c r="B686" s="5" t="s">
+        <v>1496</v>
+      </c>
+      <c r="C686" s="5" t="s">
+        <v>1497</v>
+      </c>
+      <c r="D686" s="5">
+        <v>20246422</v>
+      </c>
+      <c r="E686" s="5" t="s">
+        <v>1498</v>
+      </c>
+      <c r="F686" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G686" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H686" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I686" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="J686" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K686" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L686" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="687" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A687" s="7">
+        <v>45599.852886446759</v>
+      </c>
+      <c r="B687" s="8" t="s">
+        <v>1499</v>
+      </c>
+      <c r="C687" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="D687" s="8">
+        <v>20203702</v>
+      </c>
+      <c r="E687" s="8" t="s">
+        <v>1500</v>
+      </c>
+      <c r="F687" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G687" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H687" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="I687" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="M687" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="N687" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="O687" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="688" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A688" s="4">
+        <v>45599.855369976853</v>
+      </c>
+      <c r="B688" s="5" t="s">
+        <v>1501</v>
+      </c>
+      <c r="C688" s="5" t="s">
+        <v>1502</v>
+      </c>
+      <c r="D688" s="5">
+        <v>20206623</v>
+      </c>
+      <c r="E688" s="5" t="s">
+        <v>1503</v>
+      </c>
+      <c r="F688" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G688" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H688" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I688" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="M688" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="N688" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="O688" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="689" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A689" s="7">
+        <v>45599.857265219907</v>
+      </c>
+      <c r="B689" s="8" t="s">
+        <v>1504</v>
+      </c>
+      <c r="C689" s="8" t="s">
+        <v>1106</v>
+      </c>
+      <c r="D689" s="8">
+        <v>20193844</v>
+      </c>
+      <c r="E689" s="8" t="s">
+        <v>1505</v>
+      </c>
+      <c r="F689" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G689" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H689" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="I689" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="J689" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="K689" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="L689" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="690" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A690" s="4">
+        <v>45599.857576921291</v>
+      </c>
+      <c r="B690" s="5" t="s">
+        <v>1506</v>
+      </c>
+      <c r="C690" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="D690" s="5">
+        <v>20204103</v>
+      </c>
+      <c r="E690" s="5" t="s">
+        <v>1507</v>
+      </c>
+      <c r="F690" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G690" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H690" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I690" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="M690" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="N690" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="O690" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="691" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A691" s="7">
+        <v>45599.858236840279</v>
+      </c>
+      <c r="B691" s="8" t="s">
+        <v>1508</v>
+      </c>
+      <c r="C691" s="8" t="s">
+        <v>330</v>
+      </c>
+      <c r="D691" s="8">
+        <v>20241536</v>
+      </c>
+      <c r="E691" s="8" t="s">
+        <v>1509</v>
+      </c>
+      <c r="F691" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G691" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H691" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="I691" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="J691" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="K691" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="L691" s="8" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="692" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A692" s="4">
+        <v>45599.858616412035</v>
+      </c>
+      <c r="B692" s="5" t="s">
+        <v>1510</v>
+      </c>
+      <c r="C692" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="D692" s="5">
+        <v>20245167</v>
+      </c>
+      <c r="E692" s="5" t="s">
+        <v>1511</v>
+      </c>
+      <c r="F692" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G692" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H692" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I692" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="M692" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="N692" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="O692" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="693" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A693" s="7">
+        <v>45599.861093298612</v>
+      </c>
+      <c r="B693" s="8" t="s">
+        <v>1512</v>
+      </c>
+      <c r="C693" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="D693" s="8">
+        <v>20243803</v>
+      </c>
+      <c r="E693" s="8" t="s">
+        <v>1513</v>
+      </c>
+      <c r="F693" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G693" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H693" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="I693" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="M693" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="N693" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="O693" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="694" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A694" s="4">
+        <v>45599.864066331022</v>
+      </c>
+      <c r="B694" s="5" t="s">
+        <v>1514</v>
+      </c>
+      <c r="C694" s="5" t="s">
+        <v>403</v>
+      </c>
+      <c r="D694" s="5">
+        <v>20203523</v>
+      </c>
+      <c r="E694" s="5" t="s">
+        <v>1515</v>
+      </c>
+      <c r="F694" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G694" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H694" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I694" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="J694" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K694" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L694" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="695" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A695" s="7">
+        <v>45599.865235717589</v>
+      </c>
+      <c r="B695" s="8" t="s">
+        <v>1516</v>
+      </c>
+      <c r="C695" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="D695" s="8">
+        <v>20182923</v>
+      </c>
+      <c r="E695" s="8" t="s">
+        <v>1517</v>
+      </c>
+      <c r="F695" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G695" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="H695" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I695" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="J695" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="K695" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="L695" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="696" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A696" s="4">
+        <v>45599.869068078704</v>
+      </c>
+      <c r="B696" s="5" t="s">
+        <v>1518</v>
+      </c>
+      <c r="C696" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="D696" s="5">
+        <v>20202365</v>
+      </c>
+      <c r="E696" s="5" t="s">
+        <v>1519</v>
+      </c>
+      <c r="F696" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G696" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H696" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I696" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="J696" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K696" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="L696" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="697" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A697" s="7">
+        <v>45599.870297256944</v>
+      </c>
+      <c r="B697" s="8" t="s">
+        <v>1520</v>
+      </c>
+      <c r="C697" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="D697" s="8">
+        <v>20243636</v>
+      </c>
+      <c r="E697" s="8" t="s">
+        <v>1521</v>
+      </c>
+      <c r="F697" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G697" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="H697" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="I697" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="J697" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="K697" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="L697" s="8" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="698" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A698" s="4">
+        <v>45599.873422453704</v>
+      </c>
+      <c r="B698" s="5" t="s">
+        <v>1522</v>
+      </c>
+      <c r="C698" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D698" s="5">
+        <v>20243721</v>
+      </c>
+      <c r="E698" s="5" t="s">
+        <v>1523</v>
+      </c>
+      <c r="F698" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G698" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H698" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="I698" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="J698" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K698" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="L698" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="699" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A699" s="7">
+        <v>45599.876520347221</v>
+      </c>
+      <c r="B699" s="8" t="s">
+        <v>1524</v>
+      </c>
+      <c r="C699" s="8" t="s">
+        <v>736</v>
+      </c>
+      <c r="D699" s="8">
+        <v>20213230</v>
+      </c>
+      <c r="E699" s="8" t="s">
+        <v>1525</v>
+      </c>
+      <c r="F699" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G699" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H699" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="I699" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="M699" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="N699" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="O699" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="700" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A700" s="4">
+        <v>45599.877115578704</v>
+      </c>
+      <c r="B700" s="5" t="s">
+        <v>1526</v>
+      </c>
+      <c r="C700" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="D700" s="5">
+        <v>20233908</v>
+      </c>
+      <c r="E700" s="5" t="s">
+        <v>1527</v>
+      </c>
+      <c r="F700" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G700" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H700" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I700" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="J700" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K700" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L700" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="701" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A701" s="7">
+        <v>45599.878131273144</v>
+      </c>
+      <c r="B701" s="8" t="s">
+        <v>1528</v>
+      </c>
+      <c r="C701" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="D701" s="8">
+        <v>20233048</v>
+      </c>
+      <c r="E701" s="8" t="s">
+        <v>1529</v>
+      </c>
+      <c r="F701" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="G701" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H701" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="I701" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="M701" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="N701" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="O701" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="702" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A702" s="4">
+        <v>45599.879325671296</v>
+      </c>
+      <c r="B702" s="5" t="s">
+        <v>1530</v>
+      </c>
+      <c r="C702" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D702" s="5">
+        <v>20162755</v>
+      </c>
+      <c r="E702" s="5" t="s">
+        <v>1531</v>
+      </c>
+      <c r="F702" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G702" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H702" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="I702" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="M702" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="N702" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="O702" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="703" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A703" s="7">
+        <v>45599.879722951388</v>
+      </c>
+      <c r="B703" s="8" t="s">
+        <v>1532</v>
+      </c>
+      <c r="C703" s="8" t="s">
+        <v>330</v>
+      </c>
+      <c r="D703" s="8">
+        <v>20231532</v>
+      </c>
+      <c r="E703" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="F703" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G703" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H703" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="I703" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="M703" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="N703" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="O703" s="9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="704" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A704" s="4">
+        <v>45599.880962430558</v>
+      </c>
+      <c r="B704" s="5" t="s">
+        <v>1533</v>
+      </c>
+      <c r="C704" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D704" s="5">
+        <v>20243726</v>
+      </c>
+      <c r="E704" s="5" t="s">
+        <v>1534</v>
+      </c>
+      <c r="F704" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G704" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H704" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I704" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="J704" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="K704" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="L704" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="705" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A705" s="7">
+        <v>45599.881467754632</v>
+      </c>
+      <c r="B705" s="8" t="s">
+        <v>1535</v>
+      </c>
+      <c r="C705" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="D705" s="8">
+        <v>20222849</v>
+      </c>
+      <c r="E705" s="8" t="s">
+        <v>1536</v>
+      </c>
+      <c r="F705" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G705" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H705" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="I705" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="M705" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="N705" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="O705" s="9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="706" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A706" s="4">
+        <v>45599.881825231481</v>
+      </c>
+      <c r="B706" s="5" t="s">
+        <v>1537</v>
+      </c>
+      <c r="C706" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D706" s="5">
+        <v>20232238</v>
+      </c>
+      <c r="E706" s="5" t="s">
+        <v>1538</v>
+      </c>
+      <c r="F706" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G706" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H706" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I706" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="M706" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="N706" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="O706" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="707" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A707" s="7">
+        <v>45599.882281562503</v>
+      </c>
+      <c r="B707" s="8" t="s">
+        <v>1539</v>
+      </c>
+      <c r="C707" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="D707" s="8">
+        <v>20243844</v>
+      </c>
+      <c r="E707" s="8" t="s">
+        <v>1540</v>
+      </c>
+      <c r="F707" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G707" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H707" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="I707" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="J707" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="K707" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="L707" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="708" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A708" s="4">
+        <v>45599.882593935181</v>
+      </c>
+      <c r="B708" s="5" t="s">
+        <v>1541</v>
+      </c>
+      <c r="C708" s="5" t="s">
+        <v>1259</v>
+      </c>
+      <c r="D708" s="5">
+        <v>20232502</v>
+      </c>
+      <c r="E708" s="5" t="s">
+        <v>1542</v>
+      </c>
+      <c r="F708" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="G708" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H708" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I708" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="M708" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="N708" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="O708" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="709" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A709" s="7">
+        <v>45599.88275478009</v>
+      </c>
+      <c r="B709" s="8" t="s">
+        <v>1543</v>
+      </c>
+      <c r="C709" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="D709" s="8">
+        <v>20217103</v>
+      </c>
+      <c r="E709" s="8" t="s">
+        <v>1544</v>
+      </c>
+      <c r="F709" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G709" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="H709" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="I709" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="M709" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="N709" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="O709" s="9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="710" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A710" s="4">
+        <v>45599.885193113427</v>
+      </c>
+      <c r="B710" s="5" t="s">
+        <v>1545</v>
+      </c>
+      <c r="C710" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D710" s="5">
+        <v>20246293</v>
+      </c>
+      <c r="E710" s="5" t="s">
+        <v>1546</v>
+      </c>
+      <c r="F710" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G710" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H710" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I710" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="M710" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="N710" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="O710" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="711" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A711" s="7">
+        <v>45599.887945497685</v>
+      </c>
+      <c r="B711" s="8" t="s">
+        <v>1547</v>
+      </c>
+      <c r="C711" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D711" s="8">
+        <v>20226602</v>
+      </c>
+      <c r="E711" s="8" t="s">
+        <v>1548</v>
+      </c>
+      <c r="F711" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G711" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H711" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="I711" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="J711" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="K711" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="L711" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="712" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A712" s="4">
+        <v>45599.88933395833</v>
+      </c>
+      <c r="B712" s="5" t="s">
+        <v>1549</v>
+      </c>
+      <c r="C712" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D712" s="5">
+        <v>20202406</v>
+      </c>
+      <c r="E712" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="F712" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G712" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H712" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I712" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="J712" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="K712" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="L712" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="713" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A713" s="7">
+        <v>45599.890201539354</v>
+      </c>
+      <c r="B713" s="8" t="s">
+        <v>1550</v>
+      </c>
+      <c r="C713" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="D713" s="8">
+        <v>20242987</v>
+      </c>
+      <c r="E713" s="8" t="s">
+        <v>1551</v>
+      </c>
+      <c r="F713" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G713" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H713" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="I713" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="M713" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="N713" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="O713" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="714" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A714" s="4">
+        <v>45599.890506921292</v>
+      </c>
+      <c r="B714" s="5" t="s">
+        <v>1552</v>
+      </c>
+      <c r="C714" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="D714" s="5">
+        <v>20246770</v>
+      </c>
+      <c r="E714" s="5" t="s">
+        <v>1553</v>
+      </c>
+      <c r="F714" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="G714" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H714" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="I714" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="J714" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K714" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L714" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="715" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A715" s="7">
+        <v>45599.891241863428</v>
+      </c>
+      <c r="B715" s="8" t="s">
+        <v>1554</v>
+      </c>
+      <c r="C715" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="D715" s="8">
+        <v>20242420</v>
+      </c>
+      <c r="E715" s="8" t="s">
+        <v>1555</v>
+      </c>
+      <c r="F715" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G715" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H715" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="I715" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="M715" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="N715" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="O715" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="716" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A716" s="4">
+        <v>45599.89178283565</v>
+      </c>
+      <c r="B716" s="5" t="s">
+        <v>1556</v>
+      </c>
+      <c r="C716" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="D716" s="5">
+        <v>20192634</v>
+      </c>
+      <c r="E716" s="5" t="s">
+        <v>1557</v>
+      </c>
+      <c r="F716" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G716" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="H716" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I716" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="J716" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="K716" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L716" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="717" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A717" s="7">
+        <v>45599.89238237268</v>
+      </c>
+      <c r="B717" s="8" t="s">
+        <v>1558</v>
+      </c>
+      <c r="C717" s="8" t="s">
+        <v>315</v>
+      </c>
+      <c r="D717" s="8">
+        <v>20202849</v>
+      </c>
+      <c r="E717" s="8" t="s">
+        <v>1559</v>
+      </c>
+      <c r="F717" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G717" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H717" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="I717" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="M717" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="N717" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="O717" s="9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="718" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A718" s="4">
+        <v>45599.893887453705</v>
+      </c>
+      <c r="B718" s="5" t="s">
+        <v>1560</v>
+      </c>
+      <c r="C718" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D718" s="5">
+        <v>20213737</v>
+      </c>
+      <c r="E718" s="5" t="s">
+        <v>1561</v>
+      </c>
+      <c r="F718" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G718" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H718" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I718" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="M718" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="N718" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="O718" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="719" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A719" s="7">
+        <v>45599.894190914347</v>
+      </c>
+      <c r="B719" s="8" t="s">
+        <v>1562</v>
+      </c>
+      <c r="C719" s="8" t="s">
+        <v>1563</v>
+      </c>
+      <c r="D719" s="8">
+        <v>20216510</v>
+      </c>
+      <c r="E719" s="8" t="s">
+        <v>1564</v>
+      </c>
+      <c r="F719" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G719" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="H719" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I719" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="J719" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="K719" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="L719" s="8" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="720" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A720" s="4">
+        <v>45599.894575740742</v>
+      </c>
+      <c r="B720" s="5" t="s">
+        <v>1565</v>
+      </c>
+      <c r="C720" s="5" t="s">
+        <v>403</v>
+      </c>
+      <c r="D720" s="5">
+        <v>20203507</v>
+      </c>
+      <c r="E720" s="5" t="s">
+        <v>1566</v>
+      </c>
+      <c r="F720" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G720" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H720" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I720" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="M720" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="N720" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="O720" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="721" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A721" s="7">
+        <v>45599.895021886579</v>
+      </c>
+      <c r="B721" s="8" t="s">
+        <v>1567</v>
+      </c>
+      <c r="C721" s="8" t="s">
+        <v>330</v>
+      </c>
+      <c r="D721" s="8">
+        <v>20241509</v>
+      </c>
+      <c r="E721" s="8" t="s">
+        <v>1568</v>
+      </c>
+      <c r="F721" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G721" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H721" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="I721" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="M721" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="N721" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="O721" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="722" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A722" s="4">
+        <v>45599.89672640046</v>
+      </c>
+      <c r="B722" s="5" t="s">
+        <v>1569</v>
+      </c>
+      <c r="C722" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="D722" s="5">
+        <v>20245175</v>
+      </c>
+      <c r="E722" s="5" t="s">
+        <v>1570</v>
+      </c>
+      <c r="F722" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G722" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H722" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I722" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="M722" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="N722" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="O722" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="723" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A723" s="7">
+        <v>45599.896873495367</v>
+      </c>
+      <c r="B723" s="8" t="s">
+        <v>1571</v>
+      </c>
+      <c r="C723" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="D723" s="8">
+        <v>20246614</v>
+      </c>
+      <c r="E723" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F723" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G723" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H723" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I723" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="M723" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="N723" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="O723" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="724" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A724" s="4">
+        <v>45599.897398819448</v>
+      </c>
+      <c r="B724" s="5" t="s">
+        <v>1572</v>
+      </c>
+      <c r="C724" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D724" s="5">
+        <v>20242998</v>
+      </c>
+      <c r="E724" s="5" t="s">
+        <v>1573</v>
+      </c>
+      <c r="F724" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G724" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H724" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I724" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="J724" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K724" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L724" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="725" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A725" s="13">
+        <v>45599.899931064814</v>
+      </c>
+      <c r="B725" s="14" t="s">
+        <v>1574</v>
+      </c>
+      <c r="C725" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="D725" s="14">
+        <v>20245131</v>
+      </c>
+      <c r="E725" s="14" t="s">
+        <v>1575</v>
+      </c>
+      <c r="F725" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="G725" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="H725" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="I725" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="J725" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="K725" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="L725" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="M725" s="20"/>
+      <c r="N725" s="20"/>
+      <c r="O725" s="20"/>
+    </row>
+    <row r="726" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A726" s="4">
+        <v>45599.900814398148</v>
+      </c>
+      <c r="B726" s="5" t="s">
+        <v>1576</v>
+      </c>
+      <c r="C726" s="5" t="s">
+        <v>510</v>
+      </c>
+      <c r="D726" s="5">
+        <v>20231733</v>
+      </c>
+      <c r="E726" s="5" t="s">
+        <v>1577</v>
+      </c>
+      <c r="F726" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G726" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H726" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I726" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="M726" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="N726" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="O726" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="727" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A727" s="7">
+        <v>45599.903463391209</v>
+      </c>
+      <c r="B727" s="8" t="s">
+        <v>1578</v>
+      </c>
+      <c r="C727" s="8" t="s">
+        <v>1579</v>
+      </c>
+      <c r="D727" s="8">
+        <v>20242314</v>
+      </c>
+      <c r="E727" s="8" t="s">
+        <v>1580</v>
+      </c>
+      <c r="F727" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G727" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H727" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="I727" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="M727" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="N727" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="O727" s="9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="728" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A728" s="4">
+        <v>45599.903839803243</v>
+      </c>
+      <c r="B728" s="5" t="s">
+        <v>1581</v>
+      </c>
+      <c r="C728" s="5" t="s">
+        <v>408</v>
+      </c>
+      <c r="D728" s="5">
+        <v>20193226</v>
+      </c>
+      <c r="E728" s="5" t="s">
+        <v>1582</v>
+      </c>
+      <c r="F728" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G728" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H728" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="I728" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="J728" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="K728" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L728" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="729" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A729" s="7">
+        <v>45599.903923391204</v>
+      </c>
+      <c r="B729" s="8" t="s">
+        <v>1583</v>
+      </c>
+      <c r="C729" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="D729" s="8">
+        <v>20222122</v>
+      </c>
+      <c r="E729" s="8" t="s">
+        <v>1584</v>
+      </c>
+      <c r="F729" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="G729" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="H729" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="I729" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="J729" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="K729" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="L729" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="730" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A730" s="4">
+        <v>45599.906365509261</v>
+      </c>
+      <c r="B730" s="5" t="s">
+        <v>1585</v>
+      </c>
+      <c r="C730" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D730" s="5">
+        <v>20191623</v>
+      </c>
+      <c r="E730" s="5" t="s">
+        <v>1586</v>
+      </c>
+      <c r="F730" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G730" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H730" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I730" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="J730" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="K730" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L730" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="731" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A731" s="7">
+        <v>45599.908775856486</v>
+      </c>
+      <c r="B731" s="8" t="s">
+        <v>1587</v>
+      </c>
+      <c r="C731" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="D731" s="8">
+        <v>20233717</v>
+      </c>
+      <c r="E731" s="8" t="s">
+        <v>1588</v>
+      </c>
+      <c r="F731" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G731" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H731" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="I731" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="M731" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="N731" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="O731" s="9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="732" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A732" s="4">
+        <v>45599.909033298609</v>
+      </c>
+      <c r="B732" s="5" t="s">
+        <v>1589</v>
+      </c>
+      <c r="C732" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D732" s="5">
+        <v>20233310</v>
+      </c>
+      <c r="E732" s="5" t="s">
+        <v>1590</v>
+      </c>
+      <c r="F732" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G732" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H732" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I732" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="M732" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="N732" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="O732" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="733" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A733" s="7">
+        <v>45599.909836793981</v>
+      </c>
+      <c r="B733" s="8" t="s">
+        <v>1591</v>
+      </c>
+      <c r="C733" s="8" t="s">
+        <v>353</v>
+      </c>
+      <c r="D733" s="8">
+        <v>20233415</v>
+      </c>
+      <c r="E733" s="8" t="s">
+        <v>1592</v>
+      </c>
+      <c r="F733" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G733" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H733" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="I733" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="J733" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="K733" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="L733" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="734" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A734" s="4">
+        <v>45599.911594062505</v>
+      </c>
+      <c r="B734" s="5" t="s">
+        <v>1593</v>
+      </c>
+      <c r="C734" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="D734" s="5">
+        <v>20227103</v>
+      </c>
+      <c r="E734" s="5" t="s">
+        <v>1594</v>
+      </c>
+      <c r="F734" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="G734" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="H734" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I734" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="M734" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="N734" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="O734" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="735" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A735" s="7">
+        <v>45599.912747303242</v>
+      </c>
+      <c r="B735" s="8" t="s">
+        <v>1595</v>
+      </c>
+      <c r="C735" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="D735" s="8">
+        <v>20182850</v>
+      </c>
+      <c r="E735" s="8" t="s">
+        <v>1181</v>
+      </c>
+      <c r="F735" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="G735" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H735" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I735" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="M735" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="N735" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="O735" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="736" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A736" s="4">
+        <v>45599.913559074077</v>
+      </c>
+      <c r="B736" s="5" t="s">
+        <v>1596</v>
+      </c>
+      <c r="C736" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="D736" s="5">
+        <v>20246769</v>
+      </c>
+      <c r="E736" s="5" t="s">
+        <v>1597</v>
+      </c>
+      <c r="F736" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G736" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H736" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I736" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="M736" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="N736" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="O736" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="737" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A737" s="7">
+        <v>45599.914078611109</v>
+      </c>
+      <c r="B737" s="8" t="s">
+        <v>1598</v>
+      </c>
+      <c r="C737" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D737" s="8">
+        <v>20242511</v>
+      </c>
+      <c r="E737" s="8" t="s">
+        <v>1599</v>
+      </c>
+      <c r="F737" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G737" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="H737" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I737" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="M737" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="N737" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="O737" s="9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="738" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A738" s="4">
+        <v>45599.914261574071</v>
+      </c>
+      <c r="B738" s="5" t="s">
+        <v>1600</v>
+      </c>
+      <c r="C738" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="D738" s="5">
+        <v>20245268</v>
+      </c>
+      <c r="E738" s="5" t="s">
+        <v>1601</v>
+      </c>
+      <c r="F738" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="G738" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H738" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I738" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="M738" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="N738" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="O738" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="739" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A739" s="7">
+        <v>45599.914339328709</v>
+      </c>
+      <c r="B739" s="8" t="s">
+        <v>1602</v>
+      </c>
+      <c r="C739" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="D739" s="8">
+        <v>20243001</v>
+      </c>
+      <c r="E739" s="8" t="s">
+        <v>473</v>
+      </c>
+      <c r="F739" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G739" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="H739" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="I739" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="M739" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="N739" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="O739" s="9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="740" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A740" s="4">
+        <v>45599.914777534723</v>
+      </c>
+      <c r="B740" s="5" t="s">
+        <v>1603</v>
+      </c>
+      <c r="C740" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D740" s="5">
+        <v>20201108</v>
+      </c>
+      <c r="E740" s="5" t="s">
+        <v>1604</v>
+      </c>
+      <c r="F740" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="G740" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H740" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="I740" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="J740" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K740" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="L740" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="741" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A741" s="13">
+        <v>45599.916081342591</v>
+      </c>
+      <c r="B741" s="14" t="s">
+        <v>1605</v>
+      </c>
+      <c r="C741" s="14" t="s">
+        <v>403</v>
+      </c>
+      <c r="D741" s="14">
+        <v>20223520</v>
+      </c>
+      <c r="E741" s="14" t="s">
+        <v>1606</v>
+      </c>
+      <c r="F741" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="G741" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="H741" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="I741" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="J741" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="K741" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="L741" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="M741" s="20"/>
+      <c r="N741" s="20"/>
+      <c r="O741" s="20"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>